<commit_message>
Fix venue.id change to venue.venueId which was previously venue.providerId
</commit_message>
<xml_diff>
--- a/Data/matchDay.xlsx
+++ b/Data/matchDay.xlsx
@@ -470,7 +470,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1">
-        <v>45527</v>
+        <v>45725</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -494,7 +494,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>45549</v>
+        <v>45725</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
@@ -518,7 +518,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1">
-        <v>45548</v>
+        <v>45723</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>11</v>
@@ -566,7 +566,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1">
-        <v>45563</v>
+        <v>45723</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
UPdate based on rd 1 results
</commit_message>
<xml_diff>
--- a/Data/matchDay.xlsx
+++ b/Data/matchDay.xlsx
@@ -446,7 +446,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1">
-        <v>45528</v>
+        <v>45732</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -454,7 +454,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>45563</v>
+        <v>45731</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -462,7 +462,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1">
-        <v>45542</v>
+        <v>45729</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -470,7 +470,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1">
-        <v>45725</v>
+        <v>45731</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -478,7 +478,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
-        <v>45528</v>
+        <v>45730</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
@@ -486,7 +486,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>45529</v>
+        <v>45731</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
@@ -494,7 +494,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>45725</v>
+        <v>45732</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>45556</v>
+        <v>45731</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
@@ -510,7 +510,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1">
-        <v>45528</v>
+        <v>45732</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>10</v>
@@ -518,7 +518,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1">
-        <v>45723</v>
+        <v>45730</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>11</v>
@@ -526,7 +526,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1">
-        <v>45527</v>
+        <v>45732</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>12</v>
@@ -534,7 +534,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1">
-        <v>45528</v>
+        <v>45731</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>13</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1">
-        <v>45555</v>
+        <v>45731</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>14</v>
@@ -550,7 +550,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1">
-        <v>45528</v>
+        <v>45729</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>15</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1">
-        <v>45529</v>
+        <v>45732</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>16</v>
@@ -566,7 +566,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1">
-        <v>45723</v>
+        <v>45731</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>17</v>
@@ -574,7 +574,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1">
-        <v>45528</v>
+        <v>45732</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>18</v>
@@ -582,7 +582,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1">
-        <v>45541</v>
+        <v>45731</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Round 2 data updates
</commit_message>
<xml_diff>
--- a/Data/matchDay.xlsx
+++ b/Data/matchDay.xlsx
@@ -446,7 +446,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1">
-        <v>45732</v>
+        <v>45738</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -454,7 +454,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>45731</v>
+        <v>45739</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -462,7 +462,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1">
-        <v>45729</v>
+        <v>45736</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -470,7 +470,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1">
-        <v>45731</v>
+        <v>45737</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -478,7 +478,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
-        <v>45730</v>
+        <v>45738</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
@@ -486,7 +486,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>45731</v>
+        <v>45739</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>45731</v>
+        <v>45738</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
@@ -518,7 +518,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1">
-        <v>45730</v>
+        <v>45736</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>11</v>
@@ -526,7 +526,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1">
-        <v>45732</v>
+        <v>45739</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>12</v>
@@ -534,7 +534,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1">
-        <v>45731</v>
+        <v>45739</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>13</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1">
-        <v>45731</v>
+        <v>45738</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>14</v>
@@ -550,7 +550,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1">
-        <v>45729</v>
+        <v>45738</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>15</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1">
-        <v>45732</v>
+        <v>45738</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>16</v>
@@ -566,7 +566,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1">
-        <v>45731</v>
+        <v>45739</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>17</v>
@@ -574,7 +574,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1">
-        <v>45732</v>
+        <v>45739</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>18</v>
@@ -582,7 +582,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1">
-        <v>45731</v>
+        <v>45737</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Update with round 3 results
</commit_message>
<xml_diff>
--- a/Data/matchDay.xlsx
+++ b/Data/matchDay.xlsx
@@ -446,7 +446,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1">
-        <v>45738</v>
+        <v>45746</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -454,7 +454,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>45739</v>
+        <v>45745</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -462,7 +462,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1">
-        <v>45736</v>
+        <v>45744</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -478,7 +478,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
-        <v>45738</v>
+        <v>45743</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
@@ -486,7 +486,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>45739</v>
+        <v>45746</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
@@ -494,7 +494,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>45732</v>
+        <v>45745</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>45738</v>
+        <v>45745</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
@@ -510,7 +510,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1">
-        <v>45732</v>
+        <v>45745</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>10</v>
@@ -518,7 +518,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1">
-        <v>45736</v>
+        <v>45745</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>11</v>
@@ -526,7 +526,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1">
-        <v>45739</v>
+        <v>45745</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>12</v>
@@ -534,7 +534,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1">
-        <v>45739</v>
+        <v>45746</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>13</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1">
-        <v>45738</v>
+        <v>45743</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>14</v>
@@ -550,7 +550,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1">
-        <v>45738</v>
+        <v>45745</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>15</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1">
-        <v>45738</v>
+        <v>45745</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>16</v>
@@ -574,7 +574,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1">
-        <v>45739</v>
+        <v>45746</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>18</v>
@@ -582,7 +582,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1">
-        <v>45737</v>
+        <v>45744</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
data update after round 5
</commit_message>
<xml_diff>
--- a/Data/matchDay.xlsx
+++ b/Data/matchDay.xlsx
@@ -446,7 +446,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1">
-        <v>45891</v>
+        <v>45757</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -454,7 +454,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>45891</v>
+        <v>45759</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -462,7 +462,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1">
-        <v>45891</v>
+        <v>45759</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -470,7 +470,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1">
-        <v>45891</v>
+        <v>45758</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -478,7 +478,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
-        <v>45891</v>
+        <v>45759</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
@@ -486,7 +486,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>45891</v>
+        <v>45760</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
@@ -494,7 +494,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>45891</v>
+        <v>45760</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>45891</v>
+        <v>45757</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
@@ -510,7 +510,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1">
-        <v>45891</v>
+        <v>45759</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>10</v>
@@ -518,7 +518,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1">
-        <v>45891</v>
+        <v>45760</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>11</v>
@@ -526,7 +526,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1">
-        <v>45891</v>
+        <v>45759</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>12</v>
@@ -534,7 +534,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1">
-        <v>45891</v>
+        <v>45759</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>13</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1">
-        <v>45891</v>
+        <v>45760</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>14</v>
@@ -550,7 +550,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1">
-        <v>45891</v>
+        <v>45760</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>15</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1">
-        <v>45891</v>
+        <v>45760</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>16</v>
@@ -566,7 +566,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1">
-        <v>45891</v>
+        <v>45758</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>17</v>
@@ -574,7 +574,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1">
-        <v>45891</v>
+        <v>45759</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>18</v>
@@ -582,7 +582,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1">
-        <v>45891</v>
+        <v>45759</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Update After Round 7
</commit_message>
<xml_diff>
--- a/Data/matchDay.xlsx
+++ b/Data/matchDay.xlsx
@@ -446,7 +446,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1">
-        <v>45766</v>
+        <v>45772</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -454,7 +454,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>45764</v>
+        <v>45773</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -462,7 +462,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1">
-        <v>45765</v>
+        <v>45774</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -470,7 +470,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1">
-        <v>45764</v>
+        <v>45772</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -478,7 +478,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
-        <v>45765</v>
+        <v>45772</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
@@ -486,7 +486,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>45766</v>
+        <v>45772</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
@@ -494,7 +494,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>45766</v>
+        <v>45773</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>45768</v>
+        <v>45774</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
@@ -510,7 +510,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1">
-        <v>45766</v>
+        <v>45774</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>10</v>
@@ -518,7 +518,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1">
-        <v>45768</v>
+        <v>45774</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>11</v>
@@ -526,7 +526,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1">
-        <v>45766</v>
+        <v>45771</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>12</v>
@@ -534,7 +534,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1">
-        <v>45765</v>
+        <v>45773</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>13</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1">
-        <v>45767</v>
+        <v>45773</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>14</v>
@@ -550,7 +550,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1">
-        <v>45766</v>
+        <v>45771</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>15</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1">
-        <v>45767</v>
+        <v>45773</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>16</v>
@@ -566,7 +566,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1">
-        <v>45767</v>
+        <v>45774</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>17</v>
@@ -574,7 +574,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1">
-        <v>45765</v>
+        <v>45774</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>18</v>
@@ -582,7 +582,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1">
-        <v>45767</v>
+        <v>45773</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Updates for round 8 & round 9 tips
</commit_message>
<xml_diff>
--- a/Data/matchDay.xlsx
+++ b/Data/matchDay.xlsx
@@ -446,7 +446,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1">
-        <v>45772</v>
+        <v>45780</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -454,7 +454,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>45773</v>
+        <v>45781</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -462,7 +462,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1">
-        <v>45774</v>
+        <v>45780</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -470,7 +470,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1">
-        <v>45772</v>
+        <v>45780</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -478,7 +478,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
-        <v>45772</v>
+        <v>45778</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
@@ -486,7 +486,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>45772</v>
+        <v>45779</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
@@ -494,7 +494,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>45773</v>
+        <v>45781</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>45774</v>
+        <v>45780</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
@@ -510,7 +510,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1">
-        <v>45774</v>
+        <v>45781</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>10</v>
@@ -518,7 +518,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1">
-        <v>45774</v>
+        <v>45781</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>11</v>
@@ -526,7 +526,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1">
-        <v>45771</v>
+        <v>45780</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>12</v>
@@ -534,7 +534,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1">
-        <v>45773</v>
+        <v>45778</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>13</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1">
-        <v>45773</v>
+        <v>45780</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>14</v>
@@ -550,7 +550,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1">
-        <v>45771</v>
+        <v>45781</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>15</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1">
-        <v>45773</v>
+        <v>45779</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>16</v>
@@ -566,7 +566,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1">
-        <v>45774</v>
+        <v>45781</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>17</v>
@@ -574,7 +574,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1">
-        <v>45774</v>
+        <v>45780</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>18</v>
@@ -582,7 +582,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1">
-        <v>45773</v>
+        <v>45780</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Update the home advantage attribute
</commit_message>
<xml_diff>
--- a/Data/matchDay.xlsx
+++ b/Data/matchDay.xlsx
@@ -446,7 +446,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1">
-        <v>45780</v>
+        <v>45891</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -454,7 +454,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>45781</v>
+        <v>45891</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -462,7 +462,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1">
-        <v>45780</v>
+        <v>45891</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -470,7 +470,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1">
-        <v>45780</v>
+        <v>45891</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -478,7 +478,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
-        <v>45778</v>
+        <v>45891</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
@@ -486,7 +486,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>45779</v>
+        <v>45891</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
@@ -494,7 +494,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>45781</v>
+        <v>45891</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>45780</v>
+        <v>45891</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
@@ -510,7 +510,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1">
-        <v>45781</v>
+        <v>45891</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>10</v>
@@ -518,7 +518,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1">
-        <v>45781</v>
+        <v>45891</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>11</v>
@@ -526,7 +526,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1">
-        <v>45780</v>
+        <v>45891</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>12</v>
@@ -534,7 +534,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1">
-        <v>45778</v>
+        <v>45891</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>13</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1">
-        <v>45780</v>
+        <v>45891</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>14</v>
@@ -550,7 +550,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1">
-        <v>45781</v>
+        <v>45891</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>15</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1">
-        <v>45779</v>
+        <v>45891</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>16</v>
@@ -566,7 +566,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1">
-        <v>45781</v>
+        <v>45891</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>17</v>
@@ -574,7 +574,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1">
-        <v>45780</v>
+        <v>45891</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>18</v>
@@ -582,7 +582,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1">
-        <v>45780</v>
+        <v>45891</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Updated data + tips for round 10
</commit_message>
<xml_diff>
--- a/Data/matchDay.xlsx
+++ b/Data/matchDay.xlsx
@@ -446,7 +446,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1">
-        <v>45891</v>
+        <v>45787</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -454,7 +454,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>45891</v>
+        <v>45788</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -462,7 +462,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1">
-        <v>45891</v>
+        <v>45786</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -470,7 +470,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1">
-        <v>45891</v>
+        <v>45785</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -478,7 +478,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
-        <v>45891</v>
+        <v>45787</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
@@ -486,7 +486,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>45891</v>
+        <v>45785</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
@@ -494,7 +494,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>45891</v>
+        <v>45788</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>45891</v>
+        <v>45788</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
@@ -510,7 +510,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1">
-        <v>45891</v>
+        <v>45787</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>10</v>
@@ -518,7 +518,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1">
-        <v>45891</v>
+        <v>45787</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>11</v>
@@ -526,7 +526,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1">
-        <v>45891</v>
+        <v>45787</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>12</v>
@@ -534,7 +534,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1">
-        <v>45891</v>
+        <v>45788</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>13</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1">
-        <v>45891</v>
+        <v>45787</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>14</v>
@@ -550,7 +550,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1">
-        <v>45891</v>
+        <v>45788</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>15</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1">
-        <v>45891</v>
+        <v>45786</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>16</v>
@@ -566,7 +566,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1">
-        <v>45891</v>
+        <v>45787</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>17</v>
@@ -574,7 +574,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1">
-        <v>45891</v>
+        <v>45788</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>18</v>
@@ -582,7 +582,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1">
-        <v>45891</v>
+        <v>45787</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Updated with round 12
</commit_message>
<xml_diff>
--- a/Data/matchDay.xlsx
+++ b/Data/matchDay.xlsx
@@ -446,7 +446,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1">
-        <v>45794</v>
+        <v>45802</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -454,7 +454,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>45795</v>
+        <v>45801</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -462,7 +462,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1">
-        <v>45793</v>
+        <v>45801</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -470,7 +470,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1">
-        <v>45794</v>
+        <v>45801</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -478,7 +478,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
-        <v>45794</v>
+        <v>45800</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
@@ -486,7 +486,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>45794</v>
+        <v>45801</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
@@ -494,7 +494,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>45794</v>
+        <v>45801</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>45794</v>
+        <v>45799</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
@@ -510,7 +510,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1">
-        <v>45792</v>
+        <v>45802</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>10</v>
@@ -518,7 +518,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1">
-        <v>45792</v>
+        <v>45801</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>11</v>
@@ -526,7 +526,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1">
-        <v>45795</v>
+        <v>45802</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>12</v>
@@ -534,7 +534,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1">
-        <v>45795</v>
+        <v>45801</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>13</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1">
-        <v>45794</v>
+        <v>45801</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>14</v>
@@ -550,7 +550,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1">
-        <v>45795</v>
+        <v>45800</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>15</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1">
-        <v>45795</v>
+        <v>45802</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>16</v>
@@ -566,7 +566,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1">
-        <v>45793</v>
+        <v>45802</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>17</v>
@@ -574,7 +574,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1">
-        <v>45795</v>
+        <v>45802</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>18</v>
@@ -582,7 +582,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1">
-        <v>45794</v>
+        <v>45799</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Round 24 tip updates
</commit_message>
<xml_diff>
--- a/Data/matchDay.xlsx
+++ b/Data/matchDay.xlsx
@@ -446,7 +446,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1">
-        <v>45879</v>
+        <v>45885</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -454,7 +454,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>45878</v>
+        <v>45884</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -462,7 +462,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1">
-        <v>45878</v>
+        <v>45885</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -470,7 +470,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1">
-        <v>45876</v>
+        <v>45885</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -478,7 +478,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
-        <v>45877</v>
+        <v>45884</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
@@ -486,7 +486,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>45878</v>
+        <v>45884</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
@@ -494,7 +494,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>45879</v>
+        <v>45885</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>45877</v>
+        <v>45886</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
@@ -510,7 +510,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1">
-        <v>45878</v>
+        <v>45885</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>10</v>
@@ -518,7 +518,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1">
-        <v>45876</v>
+        <v>45885</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>11</v>
@@ -526,7 +526,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1">
-        <v>45879</v>
+        <v>45885</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>12</v>
@@ -534,7 +534,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1">
-        <v>45879</v>
+        <v>45886</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>13</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1">
-        <v>45878</v>
+        <v>45885</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>14</v>
@@ -550,7 +550,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1">
-        <v>45878</v>
+        <v>45886</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>15</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1">
-        <v>45878</v>
+        <v>45884</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>16</v>
@@ -566,7 +566,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1">
-        <v>45878</v>
+        <v>45886</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>17</v>
@@ -574,7 +574,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1">
-        <v>45879</v>
+        <v>45886</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>18</v>
@@ -582,7 +582,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1">
-        <v>45879</v>
+        <v>45886</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
grand final tip updates
</commit_message>
<xml_diff>
--- a/Data/matchDay.xlsx
+++ b/Data/matchDay.xlsx
@@ -454,7 +454,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>45913</v>
+        <v>45920</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -470,7 +470,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1">
-        <v>45904</v>
+        <v>45920</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>45905</v>
+        <v>45919</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
@@ -518,7 +518,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1">
-        <v>45912</v>
+        <v>45919</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>11</v>

</xml_diff>